<commit_message>
Store Skills,Applicants,ApplicantsSkills, JobOffers and JobOffersSkills to Db
</commit_message>
<xml_diff>
--- a/data for rs-api.xlsx
+++ b/data for rs-api.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dimitris\Desktop\codehub\01. springAcademy-Jan2020\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ilianapapadimitriou/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C3D356B-1C45-4670-8325-C1C34F58EAB4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{06506FC4-890C-1343-ABB9-51D67DF7098F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Applicants" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="Skills" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="71">
   <si>
     <t>Creativity</t>
   </si>
@@ -138,9 +137,6 @@
     <t>Ioannou</t>
   </si>
   <si>
-    <t>15 Lamias str.,</t>
-  </si>
-  <si>
     <t>Georgios</t>
   </si>
   <si>
@@ -153,27 +149,18 @@
     <t>Accenture</t>
   </si>
   <si>
-    <t>AthensJunior</t>
-  </si>
-  <si>
     <t>Mid</t>
   </si>
   <si>
     <t>Senior</t>
   </si>
   <si>
-    <t>7 Fokidos str.,</t>
-  </si>
-  <si>
     <t>Nikolaos</t>
   </si>
   <si>
     <t>Nikolaou</t>
   </si>
   <si>
-    <t>6 Fthiotidos str.,</t>
-  </si>
-  <si>
     <t>Petros</t>
   </si>
   <si>
@@ -189,9 +176,6 @@
     <t>Filippou</t>
   </si>
   <si>
-    <t>2 Artas str.,</t>
-  </si>
-  <si>
     <t>Dionyssios</t>
   </si>
   <si>
@@ -213,9 +197,6 @@
     <t>Dimou</t>
   </si>
   <si>
-    <t>4 Evrytanias str.,</t>
-  </si>
-  <si>
     <t>React</t>
   </si>
   <si>
@@ -250,6 +231,21 @@
   </si>
   <si>
     <t>Junior</t>
+  </si>
+  <si>
+    <t>15 Lamias str.</t>
+  </si>
+  <si>
+    <t>7 Fokidos str.</t>
+  </si>
+  <si>
+    <t>6 Fthiotidos str.</t>
+  </si>
+  <si>
+    <t>2 Artas str.</t>
+  </si>
+  <si>
+    <t>4 Evrytanias str.</t>
   </si>
 </sst>
 </file>
@@ -298,7 +294,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -314,7 +310,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Θέμα του Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -612,24 +608,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.1640625" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -646,7 +642,7 @@
         <v>19</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>20</v>
@@ -658,7 +654,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -675,7 +671,7 @@
         <v>30</v>
       </c>
       <c r="F2" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="G2" t="s">
         <v>11</v>
@@ -687,7 +683,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -695,7 +691,7 @@
         <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="D3" t="s">
         <v>31</v>
@@ -704,7 +700,7 @@
         <v>29</v>
       </c>
       <c r="F3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="G3" t="s">
         <v>6</v>
@@ -713,15 +709,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" t="s">
         <v>35</v>
       </c>
-      <c r="B4" t="s">
-        <v>36</v>
-      </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="D4" t="s">
         <v>31</v>
@@ -730,7 +726,7 @@
         <v>29</v>
       </c>
       <c r="F4" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="G4" t="s">
         <v>22</v>
@@ -739,15 +735,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D5" t="s">
         <v>31</v>
@@ -756,21 +752,21 @@
         <v>29</v>
       </c>
       <c r="F5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" t="s">
         <v>41</v>
       </c>
-      <c r="G5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" t="s">
-        <v>44</v>
-      </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="D6" t="s">
         <v>31</v>
@@ -779,7 +775,7 @@
         <v>29</v>
       </c>
       <c r="F6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G6" t="s">
         <v>6</v>
@@ -788,15 +784,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D7" t="s">
         <v>31</v>
@@ -805,7 +801,7 @@
         <v>29</v>
       </c>
       <c r="F7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G7" t="s">
         <v>6</v>
@@ -814,15 +810,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C8" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="D8" t="s">
         <v>31</v>
@@ -831,21 +827,21 @@
         <v>29</v>
       </c>
       <c r="F8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C9" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D9" t="s">
         <v>31</v>
@@ -854,24 +850,24 @@
         <v>29</v>
       </c>
       <c r="F9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G9" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C10" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="D10" t="s">
         <v>31</v>
@@ -880,10 +876,10 @@
         <v>29</v>
       </c>
       <c r="F10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G10" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -897,21 +893,21 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>21</v>
@@ -929,15 +925,18 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
         <v>65</v>
-      </c>
-      <c r="C2" t="s">
-        <v>39</v>
       </c>
       <c r="E2" t="s">
         <v>22</v>
@@ -946,15 +945,18 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>65</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
@@ -963,18 +965,18 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
         <v>38</v>
-      </c>
-      <c r="B4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" t="s">
-        <v>40</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
@@ -983,38 +985,38 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" t="s">
         <v>39</v>
-      </c>
-      <c r="D5" t="s">
-        <v>41</v>
       </c>
       <c r="E5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
         <v>39</v>
       </c>
-      <c r="D6" t="s">
-        <v>41</v>
-      </c>
       <c r="E6" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1026,123 +1028,123 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>